<commit_message>
update for email export RMI service
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/export/accesscnt-daily-bymachine.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/export/accesscnt-daily-bymachine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -291,22 +291,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moduleCnName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>智优</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>provided</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>crm_tomcat_pss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>moduleCnName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>智优</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>provided</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -707,7 +708,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -839,6 +840,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1224,11 +1228,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="38055296"/>
-        <c:axId val="38544512"/>
+        <c:axId val="77642752"/>
+        <c:axId val="82518784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38055296"/>
+        <c:axId val="77642752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,14 +1241,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38544512"/>
+        <c:crossAx val="82518784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38544512"/>
+        <c:axId val="82518784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1253,14 +1257,13 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38055296"/>
+        <c:crossAx val="77642752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1271,7 +1274,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001321" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001321" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001332" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001332" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1350,7 +1353,6 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G12" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A8:G12"/>
   <tableColumns count="7">
     <tableColumn id="1" name="参数" dataDxfId="6"/>
     <tableColumn id="2" name="名称" dataDxfId="5"/>
@@ -1859,7 +1861,7 @@
     </row>
     <row r="37" spans="14:14">
       <c r="N37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1901,7 +1903,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1983,8 +1985,8 @@
         <v>45</v>
       </c>
       <c r="C9" s="4" t="str">
-        <f>"["&amp;$C10&amp;"]"&amp;trend!$B24&amp;" -"&amp;$C12</f>
-        <v>[智优]服务器维度日访问量数据表 -</v>
+        <f ca="1">"["&amp;$C10&amp;"]"&amp;trend!$B24&amp;" -"&amp;$C12</f>
+        <v>[智优]服务器维度日访问量数据表 -2012-12-13</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="12"/>
@@ -1994,13 +1996,13 @@
     <row r="10" spans="1:7">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="23"/>
@@ -2014,7 +2016,7 @@
         <v>49</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>50</v>
@@ -2030,7 +2032,10 @@
       <c r="B12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="44" t="str">
+        <f ca="1">TEXT(TODAY()-1,"yyyy-mm-dd")</f>
+        <v>2012-12-13</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>46</v>
       </c>
@@ -2058,7 +2063,7 @@
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>

</xml_diff>